<commit_message>
Add new pribors, fix, refactoring
</commit_message>
<xml_diff>
--- a/Shablon/34470A.xlsx
+++ b/Shablon/34470A.xlsx
@@ -12,14 +12,23 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$H$349</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$H$350</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="389">
+  <si>
+    <t>АО "Гос МКБ "Вымпел" им. И.И. Торопова"</t>
+  </si>
+  <si>
+    <t>125424, г.Москва, Волоколамское шоссе, дом 90, стр. 23</t>
+  </si>
+  <si>
+    <t>Тел.+7 (495) 491-05-31, 22-68, e-mail: ogmetr@vympelmkb.com</t>
+  </si>
   <si>
     <t>Условия проведения калибровки:</t>
   </si>
@@ -1229,7 +1238,16 @@
     <t>Предел, В</t>
   </si>
   <si>
-    <t>TITLE</t>
+    <t>СГМетр, лаборатория средств электрических и радиотехнических измерений</t>
+  </si>
+  <si>
+    <t>Уникальный номер об аккредитации в реестре акредитованных лиц № РОСС СОБ 3.00231.2014</t>
+  </si>
+  <si>
+    <t>Заключение:</t>
+  </si>
+  <si>
+    <t>годен</t>
   </si>
 </sst>
 </file>
@@ -1544,7 +1562,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1911,6 +1929,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Денежный" xfId="1" builtinId="4"/>
@@ -2216,10 +2235,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I340"/>
+  <dimension ref="A1:I338"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:H4"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="E346" sqref="E346"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2232,7 +2251,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="110"/>
+      <c r="A1" s="110" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="110"/>
       <c r="C1" s="110"/>
       <c r="D1" s="110"/>
@@ -2243,7 +2264,9 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="110"/>
+      <c r="A2" s="110" t="s">
+        <v>385</v>
+      </c>
       <c r="B2" s="110"/>
       <c r="C2" s="110"/>
       <c r="D2" s="110"/>
@@ -2255,7 +2278,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>382</v>
+        <v>1</v>
       </c>
       <c r="B3" s="110"/>
       <c r="C3" s="110"/>
@@ -2267,7 +2290,9 @@
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="106"/>
+      <c r="A4" s="106" t="s">
+        <v>386</v>
+      </c>
       <c r="B4" s="106"/>
       <c r="C4" s="106"/>
       <c r="D4" s="106"/>
@@ -2278,7 +2303,9 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="106"/>
+      <c r="A5" s="106" t="s">
+        <v>2</v>
+      </c>
       <c r="B5" s="106"/>
       <c r="C5" s="106"/>
       <c r="D5" s="106"/>
@@ -2301,7 +2328,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="108" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="B7" s="108"/>
       <c r="C7" s="108"/>
@@ -2325,16 +2352,16 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="109" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B9" s="109"/>
       <c r="C9" s="109"/>
       <c r="D9" s="48" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E9" s="49"/>
       <c r="F9" s="50" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G9" s="50"/>
       <c r="H9" s="51"/>
@@ -2342,12 +2369,12 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="109" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B10" s="109"/>
       <c r="C10" s="109"/>
       <c r="D10" s="52" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E10" s="49"/>
       <c r="F10" s="49"/>
@@ -2357,7 +2384,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="109" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B11" s="109"/>
       <c r="C11" s="109"/>
@@ -2370,7 +2397,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="109" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B12" s="109"/>
       <c r="C12" s="109"/>
@@ -2382,12 +2409,12 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="109" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B13" s="109"/>
       <c r="C13" s="109"/>
       <c r="D13" s="52" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="E13" s="49"/>
       <c r="F13" s="49"/>
@@ -2397,12 +2424,12 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="109" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B14" s="109"/>
       <c r="C14" s="109"/>
       <c r="D14" s="54" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E14" s="49"/>
       <c r="F14" s="49"/>
@@ -2412,12 +2439,12 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="109" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B15" s="109"/>
       <c r="C15" s="109"/>
       <c r="D15" s="48" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E15" s="49"/>
       <c r="F15" s="49"/>
@@ -2430,97 +2457,97 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="115" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B18" s="116"/>
       <c r="C18" s="117"/>
       <c r="D18" s="111" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E18" s="111"/>
       <c r="F18" s="111" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G18" s="111"/>
       <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="118" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B19" s="119"/>
       <c r="C19" s="120"/>
       <c r="D19" s="112" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E19" s="112"/>
       <c r="F19" s="115" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G19" s="117"/>
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="121" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B20" s="121"/>
       <c r="C20" s="121"/>
       <c r="D20" s="112" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E20" s="112"/>
       <c r="F20" s="115" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G20" s="117"/>
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="118" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B21" s="119"/>
       <c r="C21" s="120"/>
       <c r="D21" s="113" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E21" s="114"/>
       <c r="F21" s="115" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G21" s="117"/>
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="118" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B22" s="119"/>
       <c r="C22" s="120"/>
       <c r="D22" s="122"/>
       <c r="E22" s="123"/>
       <c r="F22" s="115" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G22" s="117"/>
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="118" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B23" s="119"/>
       <c r="C23" s="120"/>
       <c r="D23" s="122"/>
       <c r="E23" s="123"/>
       <c r="F23" s="115" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G23" s="117"/>
       <c r="H23" s="10"/>
@@ -2537,7 +2564,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B25" s="46"/>
       <c r="C25" s="46"/>
@@ -2559,17 +2586,17 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -2582,7 +2609,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -2595,18 +2622,18 @@
     </row>
     <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="91" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="B31" s="85" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C31" s="86"/>
       <c r="D31" s="85" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="E31" s="86"/>
       <c r="F31" s="89" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="G31" s="90"/>
       <c r="I31" s="13"/>
@@ -2618,28 +2645,28 @@
       <c r="D32" s="87"/>
       <c r="E32" s="88"/>
       <c r="F32" s="58" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="G32" s="58" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="I32" s="13"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="91" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="B33" s="63">
         <v>10</v>
       </c>
       <c r="C33" s="101" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="D33" s="55" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E33" s="101" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="F33" s="75">
         <f>B33-0.0039</f>
@@ -2658,7 +2685,7 @@
       </c>
       <c r="C34" s="102"/>
       <c r="D34" s="55" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E34" s="102"/>
       <c r="F34" s="75">
@@ -2678,7 +2705,7 @@
       </c>
       <c r="C35" s="102"/>
       <c r="D35" s="55" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E35" s="102"/>
       <c r="F35" s="18">
@@ -2698,7 +2725,7 @@
       </c>
       <c r="C36" s="102"/>
       <c r="D36" s="55" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E36" s="102"/>
       <c r="F36" s="75">
@@ -2718,7 +2745,7 @@
       </c>
       <c r="C37" s="103"/>
       <c r="D37" s="55" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E37" s="103"/>
       <c r="F37" s="75">
@@ -2733,19 +2760,19 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="91" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="B38" s="19">
         <v>0.1</v>
       </c>
       <c r="C38" s="101" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D38" s="55" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E38" s="101" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="F38" s="64">
         <f>B38-0.000006</f>
@@ -2764,7 +2791,7 @@
       </c>
       <c r="C39" s="102"/>
       <c r="D39" s="55" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E39" s="102"/>
       <c r="F39" s="65">
@@ -2784,7 +2811,7 @@
       </c>
       <c r="C40" s="102"/>
       <c r="D40" s="55" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E40" s="102"/>
       <c r="F40" s="64">
@@ -2804,7 +2831,7 @@
       </c>
       <c r="C41" s="102"/>
       <c r="D41" s="55" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E41" s="102"/>
       <c r="F41" s="64">
@@ -2824,7 +2851,7 @@
       </c>
       <c r="C42" s="103"/>
       <c r="D42" s="55" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E42" s="103"/>
       <c r="F42" s="64">
@@ -2839,19 +2866,19 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="91" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="B43" s="63">
         <v>1</v>
       </c>
       <c r="C43" s="101" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D43" s="55" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E43" s="101" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="F43" s="65">
         <f>B43-0.000036</f>
@@ -2870,7 +2897,7 @@
       </c>
       <c r="C44" s="102"/>
       <c r="D44" s="55" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E44" s="102"/>
       <c r="F44" s="65">
@@ -2890,7 +2917,7 @@
       </c>
       <c r="C45" s="102"/>
       <c r="D45" s="55" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E45" s="102"/>
       <c r="F45" s="16">
@@ -2910,7 +2937,7 @@
       </c>
       <c r="C46" s="102"/>
       <c r="D46" s="55" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E46" s="102"/>
       <c r="F46" s="65">
@@ -2930,7 +2957,7 @@
       </c>
       <c r="C47" s="103"/>
       <c r="D47" s="55" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E47" s="103"/>
       <c r="F47" s="65">
@@ -2945,19 +2972,19 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="91" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="B48" s="63">
         <v>10</v>
       </c>
       <c r="C48" s="101" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D48" s="55" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E48" s="101" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="F48" s="18">
         <f>B48-0.00098</f>
@@ -2976,7 +3003,7 @@
       </c>
       <c r="C49" s="102"/>
       <c r="D49" s="55" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E49" s="102"/>
       <c r="F49" s="16">
@@ -2996,7 +3023,7 @@
       </c>
       <c r="C50" s="102"/>
       <c r="D50" s="55" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E50" s="102"/>
       <c r="F50" s="16">
@@ -3016,7 +3043,7 @@
       </c>
       <c r="C51" s="102"/>
       <c r="D51" s="55" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E51" s="102"/>
       <c r="F51" s="16">
@@ -3036,7 +3063,7 @@
       </c>
       <c r="C52" s="103"/>
       <c r="D52" s="55" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E52" s="103"/>
       <c r="F52" s="16">
@@ -3051,19 +3078,19 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="107" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="B53" s="63">
         <v>100</v>
       </c>
       <c r="C53" s="101" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D53" s="55" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E53" s="101" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="F53" s="15">
         <f>B53-0.0098</f>
@@ -3082,7 +3109,7 @@
       </c>
       <c r="C54" s="102"/>
       <c r="D54" s="55" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E54" s="102"/>
       <c r="F54" s="18">
@@ -3102,7 +3129,7 @@
       </c>
       <c r="C55" s="102"/>
       <c r="D55" s="55" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E55" s="102"/>
       <c r="F55" s="18">
@@ -3122,7 +3149,7 @@
       </c>
       <c r="C56" s="102"/>
       <c r="D56" s="55" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E56" s="102"/>
       <c r="F56" s="18">
@@ -3142,7 +3169,7 @@
       </c>
       <c r="C57" s="103"/>
       <c r="D57" s="55" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E57" s="103"/>
       <c r="F57" s="18">
@@ -3157,7 +3184,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
@@ -3169,21 +3196,21 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="104" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="B60" s="91" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C60" s="91"/>
       <c r="D60" s="91" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E60" s="91" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="F60" s="91"/>
       <c r="G60" s="89" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="H60" s="90"/>
     </row>
@@ -3195,30 +3222,30 @@
       <c r="E61" s="91"/>
       <c r="F61" s="91"/>
       <c r="G61" s="62" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="H61" s="62" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="79" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="B62" s="79">
         <v>10</v>
       </c>
       <c r="C62" s="82" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="D62" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E62" s="55" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F62" s="82" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="G62" s="69">
         <f>$B$62-0.025</f>
@@ -3234,10 +3261,10 @@
       <c r="B63" s="80"/>
       <c r="C63" s="83"/>
       <c r="D63" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E63" s="55" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F63" s="83"/>
       <c r="G63" s="69">
@@ -3254,10 +3281,10 @@
       <c r="B64" s="80"/>
       <c r="C64" s="83"/>
       <c r="D64" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E64" s="55" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F64" s="83"/>
       <c r="G64" s="69">
@@ -3274,10 +3301,10 @@
       <c r="B65" s="80"/>
       <c r="C65" s="83"/>
       <c r="D65" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E65" s="55" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F65" s="83"/>
       <c r="G65" s="69">
@@ -3294,10 +3321,10 @@
       <c r="B66" s="81"/>
       <c r="C66" s="84"/>
       <c r="D66" s="69" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E66" s="55" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F66" s="84"/>
       <c r="G66" s="69">
@@ -3315,16 +3342,16 @@
         <v>30</v>
       </c>
       <c r="C67" s="82" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="D67" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E67" s="55" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F67" s="82" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="G67" s="69">
         <f>$B$67-0.035</f>
@@ -3340,10 +3367,10 @@
       <c r="B68" s="80"/>
       <c r="C68" s="83"/>
       <c r="D68" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E68" s="55" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F68" s="83"/>
       <c r="G68" s="69">
@@ -3360,10 +3387,10 @@
       <c r="B69" s="80"/>
       <c r="C69" s="83"/>
       <c r="D69" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E69" s="55" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F69" s="83"/>
       <c r="G69" s="69">
@@ -3380,10 +3407,10 @@
       <c r="B70" s="80"/>
       <c r="C70" s="83"/>
       <c r="D70" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E70" s="55" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F70" s="83"/>
       <c r="G70" s="69">
@@ -3400,10 +3427,10 @@
       <c r="B71" s="81"/>
       <c r="C71" s="84"/>
       <c r="D71" s="69" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E71" s="55" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F71" s="84"/>
       <c r="G71" s="69">
@@ -3421,16 +3448,16 @@
         <v>50</v>
       </c>
       <c r="C72" s="82" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="D72" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E72" s="55" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F72" s="82" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="G72" s="69">
         <f>$B$72-0.045</f>
@@ -3446,10 +3473,10 @@
       <c r="B73" s="80"/>
       <c r="C73" s="83"/>
       <c r="D73" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E73" s="55" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="F73" s="83"/>
       <c r="G73" s="69">
@@ -3466,10 +3493,10 @@
       <c r="B74" s="80"/>
       <c r="C74" s="83"/>
       <c r="D74" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E74" s="55" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F74" s="83"/>
       <c r="G74" s="69">
@@ -3486,10 +3513,10 @@
       <c r="B75" s="80"/>
       <c r="C75" s="83"/>
       <c r="D75" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E75" s="55" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F75" s="83"/>
       <c r="G75" s="69">
@@ -3506,10 +3533,10 @@
       <c r="B76" s="81"/>
       <c r="C76" s="84"/>
       <c r="D76" s="69" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E76" s="55" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F76" s="84"/>
       <c r="G76" s="69">
@@ -3527,16 +3554,16 @@
         <v>70</v>
       </c>
       <c r="C77" s="99" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="D77" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E77" s="55" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F77" s="99" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="G77" s="69">
         <f>$B$77-0.055</f>
@@ -3552,10 +3579,10 @@
       <c r="B78" s="100"/>
       <c r="C78" s="99"/>
       <c r="D78" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E78" s="55" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F78" s="99"/>
       <c r="G78" s="69">
@@ -3572,10 +3599,10 @@
       <c r="B79" s="100"/>
       <c r="C79" s="99"/>
       <c r="D79" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E79" s="55" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F79" s="99"/>
       <c r="G79" s="69">
@@ -3592,10 +3619,10 @@
       <c r="B80" s="100"/>
       <c r="C80" s="99"/>
       <c r="D80" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E80" s="55" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F80" s="99"/>
       <c r="G80" s="69">
@@ -3612,10 +3639,10 @@
       <c r="B81" s="100"/>
       <c r="C81" s="99"/>
       <c r="D81" s="69" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E81" s="55" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F81" s="99"/>
       <c r="G81" s="69">
@@ -3633,16 +3660,16 @@
         <v>0.1</v>
       </c>
       <c r="C82" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D82" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E82" s="55" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F82" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G82" s="69">
         <f>$B$82-0.00007</f>
@@ -3658,10 +3685,10 @@
       <c r="B83" s="100"/>
       <c r="C83" s="99"/>
       <c r="D83" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E83" s="55" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F83" s="99"/>
       <c r="G83" s="69">
@@ -3678,10 +3705,10 @@
       <c r="B84" s="100"/>
       <c r="C84" s="99"/>
       <c r="D84" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E84" s="55" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F84" s="99"/>
       <c r="G84" s="69">
@@ -3698,10 +3725,10 @@
       <c r="B85" s="100"/>
       <c r="C85" s="99"/>
       <c r="D85" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E85" s="55" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F85" s="99"/>
       <c r="G85" s="69">
@@ -3718,10 +3745,10 @@
       <c r="B86" s="100"/>
       <c r="C86" s="99"/>
       <c r="D86" s="69" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E86" s="55" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F86" s="99"/>
       <c r="G86" s="69">
@@ -3735,22 +3762,22 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="79" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="B87" s="79">
         <v>0.1</v>
       </c>
       <c r="C87" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D87" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E87" s="55" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F87" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G87" s="77">
         <f>$B$87-0.00025</f>
@@ -3766,10 +3793,10 @@
       <c r="B88" s="80"/>
       <c r="C88" s="99"/>
       <c r="D88" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E88" s="55" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F88" s="99"/>
       <c r="G88" s="77">
@@ -3786,10 +3813,10 @@
       <c r="B89" s="80"/>
       <c r="C89" s="99"/>
       <c r="D89" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E89" s="55" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F89" s="99"/>
       <c r="G89" s="77">
@@ -3806,10 +3833,10 @@
       <c r="B90" s="80"/>
       <c r="C90" s="99"/>
       <c r="D90" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E90" s="55" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F90" s="99"/>
       <c r="G90" s="77">
@@ -3826,10 +3853,10 @@
       <c r="B91" s="81"/>
       <c r="C91" s="99"/>
       <c r="D91" s="69" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E91" s="55" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F91" s="99"/>
       <c r="G91" s="72">
@@ -3847,16 +3874,16 @@
         <v>0.3</v>
       </c>
       <c r="C92" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D92" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E92" s="55" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F92" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G92" s="69">
         <f>$B$92-0.00035</f>
@@ -3872,10 +3899,10 @@
       <c r="B93" s="80"/>
       <c r="C93" s="99"/>
       <c r="D93" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E93" s="55" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F93" s="99"/>
       <c r="G93" s="69">
@@ -3892,10 +3919,10 @@
       <c r="B94" s="80"/>
       <c r="C94" s="99"/>
       <c r="D94" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E94" s="55" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="F94" s="99"/>
       <c r="G94" s="69">
@@ -3912,10 +3939,10 @@
       <c r="B95" s="80"/>
       <c r="C95" s="99"/>
       <c r="D95" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E95" s="55" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F95" s="99"/>
       <c r="G95" s="69">
@@ -3932,10 +3959,10 @@
       <c r="B96" s="81"/>
       <c r="C96" s="99"/>
       <c r="D96" s="69" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E96" s="55" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="F96" s="99"/>
       <c r="G96" s="69">
@@ -3953,16 +3980,16 @@
         <v>0.5</v>
       </c>
       <c r="C97" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D97" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E97" s="55" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F97" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G97" s="69">
         <f>$B$97-0.00045</f>
@@ -3978,10 +4005,10 @@
       <c r="B98" s="80"/>
       <c r="C98" s="99"/>
       <c r="D98" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E98" s="55" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F98" s="99"/>
       <c r="G98" s="69">
@@ -3998,10 +4025,10 @@
       <c r="B99" s="80"/>
       <c r="C99" s="99"/>
       <c r="D99" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E99" s="55" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F99" s="99"/>
       <c r="G99" s="69">
@@ -4018,10 +4045,10 @@
       <c r="B100" s="80"/>
       <c r="C100" s="99"/>
       <c r="D100" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E100" s="55" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F100" s="99"/>
       <c r="G100" s="69">
@@ -4038,10 +4065,10 @@
       <c r="B101" s="81"/>
       <c r="C101" s="99"/>
       <c r="D101" s="69" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E101" s="55" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F101" s="99"/>
       <c r="G101" s="69">
@@ -4059,16 +4086,16 @@
         <v>0.7</v>
       </c>
       <c r="C102" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D102" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E102" s="55" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F102" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G102" s="69">
         <f>$B$102-0.00055</f>
@@ -4084,10 +4111,10 @@
       <c r="B103" s="80"/>
       <c r="C103" s="99"/>
       <c r="D103" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E103" s="55" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="F103" s="99"/>
       <c r="G103" s="69">
@@ -4104,10 +4131,10 @@
       <c r="B104" s="80"/>
       <c r="C104" s="99"/>
       <c r="D104" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E104" s="55" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F104" s="99"/>
       <c r="G104" s="69">
@@ -4124,10 +4151,10 @@
       <c r="B105" s="80"/>
       <c r="C105" s="99"/>
       <c r="D105" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E105" s="55" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F105" s="99"/>
       <c r="G105" s="69">
@@ -4144,10 +4171,10 @@
       <c r="B106" s="81"/>
       <c r="C106" s="99"/>
       <c r="D106" s="69" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E106" s="55" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="F106" s="99"/>
       <c r="G106" s="69">
@@ -4165,16 +4192,16 @@
         <v>1</v>
       </c>
       <c r="C107" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D107" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E107" s="55" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F107" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G107" s="69">
         <f>$B$107-0.0007</f>
@@ -4190,10 +4217,10 @@
       <c r="B108" s="80"/>
       <c r="C108" s="99"/>
       <c r="D108" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E108" s="55" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F108" s="99"/>
       <c r="G108" s="69">
@@ -4210,10 +4237,10 @@
       <c r="B109" s="80"/>
       <c r="C109" s="99"/>
       <c r="D109" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E109" s="55" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F109" s="99"/>
       <c r="G109" s="69">
@@ -4230,10 +4257,10 @@
       <c r="B110" s="80"/>
       <c r="C110" s="99"/>
       <c r="D110" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E110" s="55" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F110" s="99"/>
       <c r="G110" s="69">
@@ -4250,10 +4277,10 @@
       <c r="B111" s="81"/>
       <c r="C111" s="99"/>
       <c r="D111" s="69" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E111" s="55" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F111" s="99"/>
       <c r="G111" s="69">
@@ -4267,22 +4294,22 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="79" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="B112" s="79">
         <v>1</v>
       </c>
       <c r="C112" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D112" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E112" s="55" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="F112" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G112" s="78">
         <f>$B$112-0.0025</f>
@@ -4298,10 +4325,10 @@
       <c r="B113" s="80"/>
       <c r="C113" s="99"/>
       <c r="D113" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E113" s="55" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F113" s="99"/>
       <c r="G113" s="78">
@@ -4318,10 +4345,10 @@
       <c r="B114" s="80"/>
       <c r="C114" s="99"/>
       <c r="D114" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E114" s="55" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F114" s="99"/>
       <c r="G114" s="78">
@@ -4338,10 +4365,10 @@
       <c r="B115" s="80"/>
       <c r="C115" s="99"/>
       <c r="D115" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E115" s="55" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F115" s="99"/>
       <c r="G115" s="78">
@@ -4358,10 +4385,10 @@
       <c r="B116" s="81"/>
       <c r="C116" s="99"/>
       <c r="D116" s="69" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E116" s="55" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="F116" s="99"/>
       <c r="G116" s="74">
@@ -4379,16 +4406,16 @@
         <v>3</v>
       </c>
       <c r="C117" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D117" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E117" s="55" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F117" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G117" s="69">
         <f>$B$117-0.0035</f>
@@ -4404,10 +4431,10 @@
       <c r="B118" s="80"/>
       <c r="C118" s="99"/>
       <c r="D118" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E118" s="55" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F118" s="99"/>
       <c r="G118" s="69">
@@ -4424,10 +4451,10 @@
       <c r="B119" s="80"/>
       <c r="C119" s="99"/>
       <c r="D119" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E119" s="55" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="F119" s="99"/>
       <c r="G119" s="69">
@@ -4444,10 +4471,10 @@
       <c r="B120" s="80"/>
       <c r="C120" s="99"/>
       <c r="D120" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E120" s="55" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="F120" s="99"/>
       <c r="G120" s="69">
@@ -4464,10 +4491,10 @@
       <c r="B121" s="81"/>
       <c r="C121" s="99"/>
       <c r="D121" s="69" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E121" s="55" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="F121" s="99"/>
       <c r="G121" s="69">
@@ -4485,16 +4512,16 @@
         <v>5</v>
       </c>
       <c r="C122" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D122" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E122" s="55" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F122" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G122" s="69">
         <f>$B$122-0.0045</f>
@@ -4510,10 +4537,10 @@
       <c r="B123" s="80"/>
       <c r="C123" s="99"/>
       <c r="D123" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E123" s="55" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F123" s="99"/>
       <c r="G123" s="69">
@@ -4530,10 +4557,10 @@
       <c r="B124" s="80"/>
       <c r="C124" s="99"/>
       <c r="D124" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E124" s="55" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="F124" s="99"/>
       <c r="G124" s="69">
@@ -4550,10 +4577,10 @@
       <c r="B125" s="80"/>
       <c r="C125" s="99"/>
       <c r="D125" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E125" s="55" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="F125" s="99"/>
       <c r="G125" s="69">
@@ -4570,10 +4597,10 @@
       <c r="B126" s="81"/>
       <c r="C126" s="99"/>
       <c r="D126" s="69" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E126" s="55" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="F126" s="99"/>
       <c r="G126" s="69">
@@ -4591,16 +4618,16 @@
         <v>7</v>
       </c>
       <c r="C127" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D127" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E127" s="55" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F127" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G127" s="69">
         <f>$B$127-0.0055</f>
@@ -4616,10 +4643,10 @@
       <c r="B128" s="80"/>
       <c r="C128" s="99"/>
       <c r="D128" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E128" s="55" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F128" s="99"/>
       <c r="G128" s="69">
@@ -4636,10 +4663,10 @@
       <c r="B129" s="80"/>
       <c r="C129" s="99"/>
       <c r="D129" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E129" s="55" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F129" s="99"/>
       <c r="G129" s="69">
@@ -4656,10 +4683,10 @@
       <c r="B130" s="80"/>
       <c r="C130" s="99"/>
       <c r="D130" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E130" s="55" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="F130" s="99"/>
       <c r="G130" s="69">
@@ -4676,10 +4703,10 @@
       <c r="B131" s="81"/>
       <c r="C131" s="99"/>
       <c r="D131" s="69" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E131" s="55" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F131" s="99"/>
       <c r="G131" s="69">
@@ -4697,16 +4724,16 @@
         <v>10</v>
       </c>
       <c r="C132" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D132" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E132" s="55" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="F132" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G132" s="69">
         <f>$B$132-0.007</f>
@@ -4722,10 +4749,10 @@
       <c r="B133" s="80"/>
       <c r="C133" s="99"/>
       <c r="D133" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E133" s="55" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F133" s="99"/>
       <c r="G133" s="69">
@@ -4742,10 +4769,10 @@
       <c r="B134" s="80"/>
       <c r="C134" s="99"/>
       <c r="D134" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E134" s="55" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="F134" s="99"/>
       <c r="G134" s="69">
@@ -4762,10 +4789,10 @@
       <c r="B135" s="80"/>
       <c r="C135" s="99"/>
       <c r="D135" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E135" s="55" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F135" s="99"/>
       <c r="G135" s="69">
@@ -4782,10 +4809,10 @@
       <c r="B136" s="81"/>
       <c r="C136" s="99"/>
       <c r="D136" s="69" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E136" s="55" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="F136" s="99"/>
       <c r="G136" s="69">
@@ -4799,22 +4826,22 @@
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="79" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="B137" s="79">
         <v>10</v>
       </c>
       <c r="C137" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D137" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E137" s="55" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="F137" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G137" s="72">
         <f>$B$137-0.025</f>
@@ -4830,10 +4857,10 @@
       <c r="B138" s="80"/>
       <c r="C138" s="99"/>
       <c r="D138" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E138" s="55" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="F138" s="99"/>
       <c r="G138" s="72">
@@ -4850,10 +4877,10 @@
       <c r="B139" s="80"/>
       <c r="C139" s="99"/>
       <c r="D139" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E139" s="55" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F139" s="99"/>
       <c r="G139" s="72">
@@ -4870,10 +4897,10 @@
       <c r="B140" s="80"/>
       <c r="C140" s="99"/>
       <c r="D140" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E140" s="55" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="F140" s="99"/>
       <c r="G140" s="72">
@@ -4890,10 +4917,10 @@
       <c r="B141" s="81"/>
       <c r="C141" s="99"/>
       <c r="D141" s="69" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E141" s="55" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F141" s="99"/>
       <c r="G141" s="73">
@@ -4911,16 +4938,16 @@
         <v>30</v>
       </c>
       <c r="C142" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D142" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E142" s="55" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F142" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G142" s="69">
         <f>$B$142-0.035</f>
@@ -4936,10 +4963,10 @@
       <c r="B143" s="80"/>
       <c r="C143" s="99"/>
       <c r="D143" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E143" s="55" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F143" s="99"/>
       <c r="G143" s="69">
@@ -4956,10 +4983,10 @@
       <c r="B144" s="80"/>
       <c r="C144" s="99"/>
       <c r="D144" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E144" s="55" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="F144" s="99"/>
       <c r="G144" s="69">
@@ -4976,10 +5003,10 @@
       <c r="B145" s="80"/>
       <c r="C145" s="99"/>
       <c r="D145" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E145" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="F145" s="99"/>
       <c r="G145" s="69">
@@ -4996,10 +5023,10 @@
       <c r="B146" s="81"/>
       <c r="C146" s="99"/>
       <c r="D146" s="69" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E146" s="55" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="F146" s="99"/>
       <c r="G146" s="69">
@@ -5017,16 +5044,16 @@
         <v>50</v>
       </c>
       <c r="C147" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D147" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E147" s="55" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="F147" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G147" s="69">
         <f>$B$147-0.045</f>
@@ -5042,10 +5069,10 @@
       <c r="B148" s="80"/>
       <c r="C148" s="99"/>
       <c r="D148" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E148" s="55" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F148" s="99"/>
       <c r="G148" s="69">
@@ -5062,10 +5089,10 @@
       <c r="B149" s="80"/>
       <c r="C149" s="99"/>
       <c r="D149" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E149" s="55" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="F149" s="99"/>
       <c r="G149" s="69">
@@ -5082,10 +5109,10 @@
       <c r="B150" s="80"/>
       <c r="C150" s="99"/>
       <c r="D150" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E150" s="55" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="F150" s="99"/>
       <c r="G150" s="69">
@@ -5102,10 +5129,10 @@
       <c r="B151" s="81"/>
       <c r="C151" s="99"/>
       <c r="D151" s="69" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E151" s="55" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="F151" s="99"/>
       <c r="G151" s="69">
@@ -5123,16 +5150,16 @@
         <v>70</v>
       </c>
       <c r="C152" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D152" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E152" s="55" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F152" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G152" s="69">
         <f>$B$152-0.055</f>
@@ -5148,10 +5175,10 @@
       <c r="B153" s="80"/>
       <c r="C153" s="99"/>
       <c r="D153" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E153" s="55" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="F153" s="99"/>
       <c r="G153" s="69">
@@ -5168,10 +5195,10 @@
       <c r="B154" s="80"/>
       <c r="C154" s="99"/>
       <c r="D154" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E154" s="55" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="F154" s="99"/>
       <c r="G154" s="69">
@@ -5188,10 +5215,10 @@
       <c r="B155" s="80"/>
       <c r="C155" s="99"/>
       <c r="D155" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E155" s="55" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="F155" s="99"/>
       <c r="G155" s="69">
@@ -5208,10 +5235,10 @@
       <c r="B156" s="81"/>
       <c r="C156" s="99"/>
       <c r="D156" s="69" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E156" s="55" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F156" s="99"/>
       <c r="G156" s="69">
@@ -5229,16 +5256,16 @@
         <v>100</v>
       </c>
       <c r="C157" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D157" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E157" s="55" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F157" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G157" s="69">
         <f>$B$157-0.07</f>
@@ -5254,10 +5281,10 @@
       <c r="B158" s="80"/>
       <c r="C158" s="99"/>
       <c r="D158" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E158" s="55" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F158" s="99"/>
       <c r="G158" s="69">
@@ -5274,10 +5301,10 @@
       <c r="B159" s="80"/>
       <c r="C159" s="99"/>
       <c r="D159" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E159" s="55" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F159" s="99"/>
       <c r="G159" s="69">
@@ -5294,10 +5321,10 @@
       <c r="B160" s="80"/>
       <c r="C160" s="99"/>
       <c r="D160" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E160" s="55" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F160" s="99"/>
       <c r="G160" s="69">
@@ -5314,10 +5341,10 @@
       <c r="B161" s="81"/>
       <c r="C161" s="99"/>
       <c r="D161" s="69" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E161" s="55" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="F161" s="99"/>
       <c r="G161" s="69">
@@ -5331,22 +5358,22 @@
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="79" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="B162" s="100">
         <v>75</v>
       </c>
       <c r="C162" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D162" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E162" s="55" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="F162" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G162" s="72">
         <f>$B$162-0.1875</f>
@@ -5362,10 +5389,10 @@
       <c r="B163" s="100"/>
       <c r="C163" s="99"/>
       <c r="D163" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E163" s="55" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="F163" s="99"/>
       <c r="G163" s="72">
@@ -5382,10 +5409,10 @@
       <c r="B164" s="100"/>
       <c r="C164" s="99"/>
       <c r="D164" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E164" s="55" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F164" s="99"/>
       <c r="G164" s="72">
@@ -5403,16 +5430,16 @@
         <v>225</v>
       </c>
       <c r="C165" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D165" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E165" s="55" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F165" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G165" s="72">
         <f>$B$165-0.2625</f>
@@ -5428,10 +5455,10 @@
       <c r="B166" s="100"/>
       <c r="C166" s="99"/>
       <c r="D166" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E166" s="55" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="F166" s="99"/>
       <c r="G166" s="72">
@@ -5448,10 +5475,10 @@
       <c r="B167" s="100"/>
       <c r="C167" s="99"/>
       <c r="D167" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E167" s="55" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F167" s="99"/>
       <c r="G167" s="72">
@@ -5469,16 +5496,16 @@
         <v>375</v>
       </c>
       <c r="C168" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D168" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E168" s="55" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="F168" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G168" s="72">
         <f>$B$168-0.3375</f>
@@ -5494,10 +5521,10 @@
       <c r="B169" s="100"/>
       <c r="C169" s="99"/>
       <c r="D169" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E169" s="55" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="F169" s="99"/>
       <c r="G169" s="72">
@@ -5514,10 +5541,10 @@
       <c r="B170" s="100"/>
       <c r="C170" s="99"/>
       <c r="D170" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E170" s="55" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F170" s="99"/>
       <c r="G170" s="72">
@@ -5535,16 +5562,16 @@
         <v>525</v>
       </c>
       <c r="C171" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D171" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E171" s="55" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="F171" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G171" s="72">
         <f>$B$171-0.6375</f>
@@ -5560,10 +5587,10 @@
       <c r="B172" s="100"/>
       <c r="C172" s="99"/>
       <c r="D172" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E172" s="55" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="F172" s="99"/>
       <c r="G172" s="72">
@@ -5580,10 +5607,10 @@
       <c r="B173" s="100"/>
       <c r="C173" s="99"/>
       <c r="D173" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E173" s="55" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F173" s="99"/>
       <c r="G173" s="72">
@@ -5601,16 +5628,16 @@
         <v>750</v>
       </c>
       <c r="C174" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D174" s="69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E174" s="55" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="F174" s="99" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G174" s="72">
         <f>$B$174-0.975</f>
@@ -5626,10 +5653,10 @@
       <c r="B175" s="100"/>
       <c r="C175" s="99"/>
       <c r="D175" s="69" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E175" s="55" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="F175" s="99"/>
       <c r="G175" s="73">
@@ -5646,10 +5673,10 @@
       <c r="B176" s="100"/>
       <c r="C176" s="99"/>
       <c r="D176" s="69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E176" s="55" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="F176" s="99"/>
       <c r="G176" s="74">
@@ -5671,7 +5698,7 @@
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="26" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B178" s="21"/>
       <c r="C178" s="22"/>
@@ -5681,18 +5708,18 @@
     </row>
     <row r="179" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="91" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="B179" s="91" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C179" s="91"/>
       <c r="D179" s="91" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E179" s="91"/>
       <c r="F179" s="89" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="G179" s="90"/>
     </row>
@@ -5703,27 +5730,27 @@
       <c r="D180" s="91"/>
       <c r="E180" s="91"/>
       <c r="F180" s="58" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="G180" s="58" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="100" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="B181" s="60">
         <v>100</v>
       </c>
       <c r="C181" s="100" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="D181" s="55" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E181" s="100" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="F181" s="15">
         <f>B181-0.1</f>
@@ -5741,7 +5768,7 @@
       </c>
       <c r="C182" s="100"/>
       <c r="D182" s="55" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E182" s="100"/>
       <c r="F182" s="15">
@@ -5760,7 +5787,7 @@
       </c>
       <c r="C183" s="100"/>
       <c r="D183" s="55" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E183" s="100"/>
       <c r="F183" s="15">
@@ -5779,7 +5806,7 @@
       </c>
       <c r="C184" s="100"/>
       <c r="D184" s="55" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E184" s="100"/>
       <c r="F184" s="15">
@@ -5797,13 +5824,13 @@
         <v>1</v>
       </c>
       <c r="C185" s="60" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="D185" s="55" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="E185" s="60" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="F185" s="65">
         <f>B185-0.00055</f>
@@ -5816,19 +5843,19 @@
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="100" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B186" s="60">
         <v>1</v>
       </c>
       <c r="C186" s="79" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="D186" s="55" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E186" s="79" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="F186" s="76">
         <f>B186-0.0025</f>
@@ -5846,7 +5873,7 @@
       </c>
       <c r="C187" s="80"/>
       <c r="D187" s="55" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E187" s="80"/>
       <c r="F187" s="76">
@@ -5865,7 +5892,7 @@
       </c>
       <c r="C188" s="80"/>
       <c r="D188" s="55" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E188" s="80"/>
       <c r="F188" s="76">
@@ -5884,7 +5911,7 @@
       </c>
       <c r="C189" s="80"/>
       <c r="D189" s="55" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E189" s="80"/>
       <c r="F189" s="76">
@@ -5903,7 +5930,7 @@
       </c>
       <c r="C190" s="81"/>
       <c r="D190" s="55" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E190" s="81"/>
       <c r="F190" s="18">
@@ -5917,19 +5944,19 @@
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="100" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B191" s="60">
         <v>10</v>
       </c>
       <c r="C191" s="79" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="D191" s="55" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="E191" s="79" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="F191" s="15">
         <f>B191-0.01</f>
@@ -5947,7 +5974,7 @@
       </c>
       <c r="C192" s="80"/>
       <c r="D192" s="55" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="E192" s="80"/>
       <c r="F192" s="15">
@@ -5966,7 +5993,7 @@
       </c>
       <c r="C193" s="80"/>
       <c r="D193" s="55" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E193" s="80"/>
       <c r="F193" s="15">
@@ -5985,7 +6012,7 @@
       </c>
       <c r="C194" s="80"/>
       <c r="D194" s="55" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="E194" s="80"/>
       <c r="F194" s="15">
@@ -6004,7 +6031,7 @@
       </c>
       <c r="C195" s="81"/>
       <c r="D195" s="55" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="E195" s="81"/>
       <c r="F195" s="18">
@@ -6018,19 +6045,19 @@
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="100" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B196" s="60">
         <v>0.1</v>
       </c>
       <c r="C196" s="79" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="D196" s="55" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E196" s="79" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="F196" s="65">
         <f>B196-0.00018</f>
@@ -6048,7 +6075,7 @@
       </c>
       <c r="C197" s="80"/>
       <c r="D197" s="55" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E197" s="80"/>
       <c r="F197" s="65">
@@ -6067,7 +6094,7 @@
       </c>
       <c r="C198" s="80"/>
       <c r="D198" s="55" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="E198" s="80"/>
       <c r="F198" s="65">
@@ -6086,7 +6113,7 @@
       </c>
       <c r="C199" s="80"/>
       <c r="D199" s="55" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="E199" s="80"/>
       <c r="F199" s="65">
@@ -6105,7 +6132,7 @@
       </c>
       <c r="C200" s="81"/>
       <c r="D200" s="55" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="E200" s="81"/>
       <c r="F200" s="76">
@@ -6119,19 +6146,19 @@
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="100" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B201" s="60">
         <v>0.3</v>
       </c>
       <c r="C201" s="79" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="D201" s="55" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="E201" s="79" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="F201" s="76">
         <f>B201-0.0012</f>
@@ -6149,7 +6176,7 @@
       </c>
       <c r="C202" s="80"/>
       <c r="D202" s="55" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E202" s="80"/>
       <c r="F202" s="76">
@@ -6168,7 +6195,7 @@
       </c>
       <c r="C203" s="80"/>
       <c r="D203" s="55" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E203" s="80"/>
       <c r="F203" s="76">
@@ -6187,7 +6214,7 @@
       </c>
       <c r="C204" s="80"/>
       <c r="D204" s="55" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="E204" s="80"/>
       <c r="F204" s="76">
@@ -6206,7 +6233,7 @@
       </c>
       <c r="C205" s="81"/>
       <c r="D205" s="55" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="E205" s="81"/>
       <c r="F205" s="76">
@@ -6220,19 +6247,19 @@
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" s="100" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B206" s="60">
         <v>1</v>
       </c>
       <c r="C206" s="79" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="D206" s="55" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="E206" s="79" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="F206" s="76">
         <f>B206-0.0022</f>
@@ -6250,7 +6277,7 @@
       </c>
       <c r="C207" s="80"/>
       <c r="D207" s="55" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E207" s="80"/>
       <c r="F207" s="76">
@@ -6269,7 +6296,7 @@
       </c>
       <c r="C208" s="80"/>
       <c r="D208" s="55" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="E208" s="80"/>
       <c r="F208" s="18">
@@ -6288,7 +6315,7 @@
       </c>
       <c r="C209" s="80"/>
       <c r="D209" s="55" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="E209" s="80"/>
       <c r="F209" s="76">
@@ -6307,7 +6334,7 @@
       </c>
       <c r="C210" s="81"/>
       <c r="D210" s="55" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="E210" s="81"/>
       <c r="F210" s="18">
@@ -6329,7 +6356,7 @@
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="26" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B212" s="20"/>
       <c r="C212" s="22"/>
@@ -6339,21 +6366,21 @@
     </row>
     <row r="213" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="104" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="B213" s="91" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C213" s="91"/>
       <c r="D213" s="91" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E213" s="91" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="F213" s="91"/>
       <c r="G213" s="89" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="H213" s="90"/>
     </row>
@@ -6365,30 +6392,30 @@
       <c r="E214" s="91"/>
       <c r="F214" s="91"/>
       <c r="G214" s="62" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="H214" s="62" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="79" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B215" s="82">
         <v>100</v>
       </c>
       <c r="C215" s="82" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="D215" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E215" s="55" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="F215" s="82" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="G215" s="82">
         <f>$B$215-0.14</f>
@@ -6404,10 +6431,10 @@
       <c r="B216" s="83"/>
       <c r="C216" s="83"/>
       <c r="D216" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E216" s="55" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="F216" s="83"/>
       <c r="G216" s="83"/>
@@ -6418,10 +6445,10 @@
       <c r="B217" s="84"/>
       <c r="C217" s="84"/>
       <c r="D217" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E217" s="55" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="F217" s="84"/>
       <c r="G217" s="84"/>
@@ -6429,22 +6456,22 @@
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="79" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B218" s="82">
         <v>100</v>
       </c>
       <c r="C218" s="82" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="D218" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E218" s="55" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="F218" s="82" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="G218" s="82">
         <f>B218-0.5</f>
@@ -6460,10 +6487,10 @@
       <c r="B219" s="83"/>
       <c r="C219" s="83"/>
       <c r="D219" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E219" s="55" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="F219" s="83"/>
       <c r="G219" s="83"/>
@@ -6474,10 +6501,10 @@
       <c r="B220" s="84"/>
       <c r="C220" s="84"/>
       <c r="D220" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E220" s="55" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="F220" s="84"/>
       <c r="G220" s="84"/>
@@ -6489,16 +6516,16 @@
         <v>300</v>
       </c>
       <c r="C221" s="82" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="D221" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E221" s="55" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="F221" s="82" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="G221" s="82">
         <f>B221-0.7</f>
@@ -6514,10 +6541,10 @@
       <c r="B222" s="83"/>
       <c r="C222" s="83"/>
       <c r="D222" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E222" s="55" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="F222" s="83"/>
       <c r="G222" s="83"/>
@@ -6528,10 +6555,10 @@
       <c r="B223" s="84"/>
       <c r="C223" s="84"/>
       <c r="D223" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E223" s="55" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="F223" s="84"/>
       <c r="G223" s="84"/>
@@ -6543,16 +6570,16 @@
         <v>500</v>
       </c>
       <c r="C224" s="82" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="D224" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E224" s="55" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="F224" s="82" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="G224" s="82">
         <f>B224-0.9</f>
@@ -6568,10 +6595,10 @@
       <c r="B225" s="83"/>
       <c r="C225" s="83"/>
       <c r="D225" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E225" s="55" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="F225" s="83"/>
       <c r="G225" s="83"/>
@@ -6582,10 +6609,10 @@
       <c r="B226" s="84"/>
       <c r="C226" s="84"/>
       <c r="D226" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E226" s="55" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="F226" s="84"/>
       <c r="G226" s="84"/>
@@ -6597,16 +6624,16 @@
         <v>700</v>
       </c>
       <c r="C227" s="82" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="D227" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E227" s="55" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="F227" s="82" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="G227" s="82">
         <f>B227-1.1</f>
@@ -6622,10 +6649,10 @@
       <c r="B228" s="83"/>
       <c r="C228" s="83"/>
       <c r="D228" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E228" s="55" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="F228" s="83"/>
       <c r="G228" s="83"/>
@@ -6636,10 +6663,10 @@
       <c r="B229" s="84"/>
       <c r="C229" s="84"/>
       <c r="D229" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E229" s="55" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="F229" s="84"/>
       <c r="G229" s="84"/>
@@ -6651,16 +6678,16 @@
         <v>1</v>
       </c>
       <c r="C230" s="82" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="D230" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E230" s="55" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="F230" s="82" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="G230" s="82">
         <f>B230-0.0014</f>
@@ -6676,10 +6703,10 @@
       <c r="B231" s="83"/>
       <c r="C231" s="83"/>
       <c r="D231" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E231" s="55" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="F231" s="83"/>
       <c r="G231" s="83"/>
@@ -6690,10 +6717,10 @@
       <c r="B232" s="84"/>
       <c r="C232" s="84"/>
       <c r="D232" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E232" s="55" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="F232" s="84"/>
       <c r="G232" s="84"/>
@@ -6701,22 +6728,22 @@
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233" s="79" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B233" s="82">
         <v>1</v>
       </c>
       <c r="C233" s="82" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="D233" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E233" s="55" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="F233" s="82" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="G233" s="82">
         <f>B233-0.005</f>
@@ -6732,10 +6759,10 @@
       <c r="B234" s="83"/>
       <c r="C234" s="83"/>
       <c r="D234" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E234" s="55" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="F234" s="83"/>
       <c r="G234" s="83"/>
@@ -6746,10 +6773,10 @@
       <c r="B235" s="84"/>
       <c r="C235" s="84"/>
       <c r="D235" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E235" s="55" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F235" s="84"/>
       <c r="G235" s="84"/>
@@ -6761,16 +6788,16 @@
         <v>3</v>
       </c>
       <c r="C236" s="82" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="D236" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E236" s="55" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="F236" s="82" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="G236" s="82">
         <f>B236-0.007</f>
@@ -6786,10 +6813,10 @@
       <c r="B237" s="83"/>
       <c r="C237" s="83"/>
       <c r="D237" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E237" s="55" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="F237" s="83"/>
       <c r="G237" s="83"/>
@@ -6800,10 +6827,10 @@
       <c r="B238" s="84"/>
       <c r="C238" s="84"/>
       <c r="D238" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E238" s="55" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="F238" s="84"/>
       <c r="G238" s="84"/>
@@ -6815,16 +6842,16 @@
         <v>5</v>
       </c>
       <c r="C239" s="82" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="D239" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E239" s="55" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="F239" s="82" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="G239" s="82">
         <f>B239-0.009</f>
@@ -6840,10 +6867,10 @@
       <c r="B240" s="83"/>
       <c r="C240" s="83"/>
       <c r="D240" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E240" s="55" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="F240" s="83"/>
       <c r="G240" s="83"/>
@@ -6854,10 +6881,10 @@
       <c r="B241" s="84"/>
       <c r="C241" s="84"/>
       <c r="D241" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E241" s="55" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="F241" s="84"/>
       <c r="G241" s="84"/>
@@ -6869,16 +6896,16 @@
         <v>7</v>
       </c>
       <c r="C242" s="82" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="D242" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E242" s="55" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="F242" s="82" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="G242" s="82">
         <f>B242-0.011</f>
@@ -6894,10 +6921,10 @@
       <c r="B243" s="83"/>
       <c r="C243" s="83"/>
       <c r="D243" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E243" s="55" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="F243" s="83"/>
       <c r="G243" s="83"/>
@@ -6908,10 +6935,10 @@
       <c r="B244" s="84"/>
       <c r="C244" s="84"/>
       <c r="D244" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E244" s="55" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="F244" s="84"/>
       <c r="G244" s="84"/>
@@ -6923,16 +6950,16 @@
         <v>10</v>
       </c>
       <c r="C245" s="82" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="D245" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E245" s="55" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="F245" s="82" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="G245" s="82">
         <f>B245-0.014</f>
@@ -6948,10 +6975,10 @@
       <c r="B246" s="83"/>
       <c r="C246" s="83"/>
       <c r="D246" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E246" s="55" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="F246" s="83"/>
       <c r="G246" s="83"/>
@@ -6962,10 +6989,10 @@
       <c r="B247" s="84"/>
       <c r="C247" s="84"/>
       <c r="D247" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E247" s="55" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="F247" s="84"/>
       <c r="G247" s="84"/>
@@ -6973,22 +7000,22 @@
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" s="79" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B248" s="82">
         <v>10</v>
       </c>
       <c r="C248" s="82" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="D248" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E248" s="55" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="F248" s="82" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="G248" s="82">
         <f>B248-0.05</f>
@@ -7004,10 +7031,10 @@
       <c r="B249" s="83"/>
       <c r="C249" s="83"/>
       <c r="D249" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E249" s="55" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="F249" s="83"/>
       <c r="G249" s="83"/>
@@ -7018,10 +7045,10 @@
       <c r="B250" s="84"/>
       <c r="C250" s="84"/>
       <c r="D250" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E250" s="55" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="F250" s="84"/>
       <c r="G250" s="84"/>
@@ -7033,16 +7060,16 @@
         <v>30</v>
       </c>
       <c r="C251" s="82" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="D251" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E251" s="55" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="F251" s="82" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="G251" s="82">
         <f>B251-0.07</f>
@@ -7058,10 +7085,10 @@
       <c r="B252" s="83"/>
       <c r="C252" s="83"/>
       <c r="D252" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E252" s="55" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="F252" s="83"/>
       <c r="G252" s="83"/>
@@ -7072,10 +7099,10 @@
       <c r="B253" s="84"/>
       <c r="C253" s="84"/>
       <c r="D253" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E253" s="55" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="F253" s="84"/>
       <c r="G253" s="84"/>
@@ -7087,16 +7114,16 @@
         <v>50</v>
       </c>
       <c r="C254" s="82" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="D254" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E254" s="55" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="F254" s="82" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="G254" s="82">
         <f>B254-0.09</f>
@@ -7112,10 +7139,10 @@
       <c r="B255" s="83"/>
       <c r="C255" s="83"/>
       <c r="D255" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E255" s="55" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="F255" s="83"/>
       <c r="G255" s="83"/>
@@ -7126,10 +7153,10 @@
       <c r="B256" s="84"/>
       <c r="C256" s="84"/>
       <c r="D256" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E256" s="55" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="F256" s="84"/>
       <c r="G256" s="84"/>
@@ -7141,16 +7168,16 @@
         <v>70</v>
       </c>
       <c r="C257" s="82" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="D257" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E257" s="55" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="F257" s="82" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="G257" s="82">
         <f>B257-0.11</f>
@@ -7166,10 +7193,10 @@
       <c r="B258" s="83"/>
       <c r="C258" s="83"/>
       <c r="D258" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E258" s="55" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="F258" s="83"/>
       <c r="G258" s="83"/>
@@ -7180,10 +7207,10 @@
       <c r="B259" s="84"/>
       <c r="C259" s="84"/>
       <c r="D259" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E259" s="55" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="F259" s="84"/>
       <c r="G259" s="84"/>
@@ -7195,16 +7222,16 @@
         <v>100</v>
       </c>
       <c r="C260" s="82" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="D260" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E260" s="55" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="F260" s="82" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="G260" s="82">
         <f>B260-0.14</f>
@@ -7220,10 +7247,10 @@
       <c r="B261" s="83"/>
       <c r="C261" s="83"/>
       <c r="D261" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E261" s="55" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="F261" s="83"/>
       <c r="G261" s="83"/>
@@ -7234,10 +7261,10 @@
       <c r="B262" s="84"/>
       <c r="C262" s="84"/>
       <c r="D262" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E262" s="55" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="F262" s="84"/>
       <c r="G262" s="84"/>
@@ -7245,22 +7272,22 @@
     </row>
     <row r="263" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A263" s="79" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B263" s="82">
         <v>0.1</v>
       </c>
       <c r="C263" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="D263" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E263" s="55" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="F263" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G263" s="82">
         <f>B263-0.0005</f>
@@ -7276,10 +7303,10 @@
       <c r="B264" s="83"/>
       <c r="C264" s="83"/>
       <c r="D264" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E264" s="55" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="F264" s="83"/>
       <c r="G264" s="83"/>
@@ -7290,10 +7317,10 @@
       <c r="B265" s="84"/>
       <c r="C265" s="84"/>
       <c r="D265" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E265" s="55" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="F265" s="84"/>
       <c r="G265" s="84"/>
@@ -7305,16 +7332,16 @@
         <v>0.3</v>
       </c>
       <c r="C266" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="D266" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E266" s="55" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="F266" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G266" s="82">
         <f>B266-0.0007</f>
@@ -7330,10 +7357,10 @@
       <c r="B267" s="83"/>
       <c r="C267" s="83"/>
       <c r="D267" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E267" s="55" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="F267" s="83"/>
       <c r="G267" s="83"/>
@@ -7344,10 +7371,10 @@
       <c r="B268" s="84"/>
       <c r="C268" s="84"/>
       <c r="D268" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E268" s="55" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="F268" s="84"/>
       <c r="G268" s="84"/>
@@ -7359,16 +7386,16 @@
         <v>0.5</v>
       </c>
       <c r="C269" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="D269" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E269" s="55" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="F269" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G269" s="82">
         <f>B269-0.0009</f>
@@ -7384,10 +7411,10 @@
       <c r="B270" s="83"/>
       <c r="C270" s="83"/>
       <c r="D270" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E270" s="55" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="F270" s="83"/>
       <c r="G270" s="83"/>
@@ -7398,10 +7425,10 @@
       <c r="B271" s="84"/>
       <c r="C271" s="84"/>
       <c r="D271" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E271" s="55" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F271" s="84"/>
       <c r="G271" s="84"/>
@@ -7413,16 +7440,16 @@
         <v>0.7</v>
       </c>
       <c r="C272" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="D272" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E272" s="55" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="F272" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G272" s="82">
         <f>B272-0.0011</f>
@@ -7438,10 +7465,10 @@
       <c r="B273" s="83"/>
       <c r="C273" s="83"/>
       <c r="D273" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E273" s="55" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="F273" s="83"/>
       <c r="G273" s="83"/>
@@ -7452,10 +7479,10 @@
       <c r="B274" s="84"/>
       <c r="C274" s="84"/>
       <c r="D274" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E274" s="55" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="F274" s="84"/>
       <c r="G274" s="84"/>
@@ -7467,16 +7494,16 @@
         <v>1</v>
       </c>
       <c r="C275" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="D275" s="69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E275" s="55" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="F275" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G275" s="82">
         <f>B275-0.0014</f>
@@ -7492,10 +7519,10 @@
       <c r="B276" s="83"/>
       <c r="C276" s="83"/>
       <c r="D276" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E276" s="55" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="F276" s="83"/>
       <c r="G276" s="83"/>
@@ -7506,10 +7533,10 @@
       <c r="B277" s="84"/>
       <c r="C277" s="84"/>
       <c r="D277" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E277" s="55" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="F277" s="84"/>
       <c r="G277" s="84"/>
@@ -7517,22 +7544,22 @@
     </row>
     <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="79" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B278" s="82">
         <v>0.3</v>
       </c>
       <c r="C278" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="D278" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E278" s="55" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="F278" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G278" s="82">
         <f>B278-0.00189</f>
@@ -7548,10 +7575,10 @@
       <c r="B279" s="84"/>
       <c r="C279" s="84"/>
       <c r="D279" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E279" s="55" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="F279" s="84"/>
       <c r="G279" s="84"/>
@@ -7563,16 +7590,16 @@
         <v>0.9</v>
       </c>
       <c r="C280" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="D280" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E280" s="55" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="F280" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G280" s="82">
         <f>B280-0.00327</f>
@@ -7588,10 +7615,10 @@
       <c r="B281" s="84"/>
       <c r="C281" s="84"/>
       <c r="D281" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E281" s="55" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="F281" s="84"/>
       <c r="G281" s="84"/>
@@ -7603,16 +7630,16 @@
         <v>1.5</v>
       </c>
       <c r="C282" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="D282" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E282" s="55" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="F282" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G282" s="82">
         <f>B282-0.00465</f>
@@ -7628,10 +7655,10 @@
       <c r="B283" s="84"/>
       <c r="C283" s="84"/>
       <c r="D283" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E283" s="55" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="F283" s="84"/>
       <c r="G283" s="84"/>
@@ -7643,16 +7670,16 @@
         <v>2.1</v>
       </c>
       <c r="C284" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="D284" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E284" s="55" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="F284" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G284" s="82">
         <f>B284-0.00603</f>
@@ -7668,10 +7695,10 @@
       <c r="B285" s="84"/>
       <c r="C285" s="84"/>
       <c r="D285" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E285" s="55" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="F285" s="84"/>
       <c r="G285" s="84"/>
@@ -7683,16 +7710,16 @@
         <v>3</v>
       </c>
       <c r="C286" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="D286" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E286" s="55" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="F286" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G286" s="82">
         <f>B286-0.00801</f>
@@ -7708,10 +7735,10 @@
       <c r="B287" s="84"/>
       <c r="C287" s="84"/>
       <c r="D287" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E287" s="55" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="F287" s="84"/>
       <c r="G287" s="84"/>
@@ -7719,22 +7746,22 @@
     </row>
     <row r="288" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A288" s="79" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B288" s="82">
         <v>1</v>
       </c>
       <c r="C288" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="D288" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E288" s="55" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="F288" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G288" s="82">
         <f>B288-0.005</f>
@@ -7750,10 +7777,10 @@
       <c r="B289" s="84"/>
       <c r="C289" s="84"/>
       <c r="D289" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E289" s="55" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="F289" s="84"/>
       <c r="G289" s="84"/>
@@ -7765,16 +7792,16 @@
         <v>3</v>
       </c>
       <c r="C290" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="D290" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E290" s="55" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="F290" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G290" s="82">
         <f>B290-0.007</f>
@@ -7790,10 +7817,10 @@
       <c r="B291" s="84"/>
       <c r="C291" s="84"/>
       <c r="D291" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E291" s="55" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="F291" s="84"/>
       <c r="G291" s="84"/>
@@ -7805,16 +7832,16 @@
         <v>5</v>
       </c>
       <c r="C292" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="D292" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E292" s="55" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="F292" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G292" s="82">
         <f>B292-0.009</f>
@@ -7830,10 +7857,10 @@
       <c r="B293" s="84"/>
       <c r="C293" s="84"/>
       <c r="D293" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E293" s="55" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="F293" s="84"/>
       <c r="G293" s="84"/>
@@ -7845,16 +7872,16 @@
         <v>7</v>
       </c>
       <c r="C294" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="D294" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E294" s="55" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="F294" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G294" s="82">
         <f>B294-0.015</f>
@@ -7870,10 +7897,10 @@
       <c r="B295" s="84"/>
       <c r="C295" s="84"/>
       <c r="D295" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E295" s="55" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="F295" s="84"/>
       <c r="G295" s="84"/>
@@ -7885,16 +7912,16 @@
         <v>10</v>
       </c>
       <c r="C296" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="D296" s="69" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E296" s="55" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="F296" s="82" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G296" s="82">
         <f>B296-0.024</f>
@@ -7910,10 +7937,10 @@
       <c r="B297" s="84"/>
       <c r="C297" s="84"/>
       <c r="D297" s="69" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E297" s="55" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="F297" s="84"/>
       <c r="G297" s="84"/>
@@ -7929,7 +7956,7 @@
     </row>
     <row r="299" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A299" s="26" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B299" s="20"/>
       <c r="C299" s="20"/>
@@ -7939,21 +7966,21 @@
     </row>
     <row r="300" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A300" s="91" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="B300" s="98" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="C300" s="91" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="D300" s="91"/>
       <c r="E300" s="91" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="F300" s="91"/>
       <c r="G300" s="89" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="H300" s="90"/>
     </row>
@@ -7965,10 +7992,10 @@
       <c r="E301" s="91"/>
       <c r="F301" s="91"/>
       <c r="G301" s="59" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="H301" s="59" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="302" spans="1:8" x14ac:dyDescent="0.25">
@@ -7982,13 +8009,13 @@
         <v>5</v>
       </c>
       <c r="D302" s="82" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="E302" s="56" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="F302" s="82" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="G302" s="69">
         <f>C302-0.0035</f>
@@ -8007,7 +8034,7 @@
       </c>
       <c r="D303" s="83"/>
       <c r="E303" s="56" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="F303" s="83"/>
       <c r="G303" s="69">
@@ -8027,7 +8054,7 @@
       </c>
       <c r="D304" s="84"/>
       <c r="E304" s="56" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="F304" s="84"/>
       <c r="G304" s="69">
@@ -8046,13 +8073,13 @@
         <v>100</v>
       </c>
       <c r="D305" s="69" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="E305" s="56" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F305" s="69" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="G305" s="69">
         <f>C305-0.007</f>
@@ -8074,13 +8101,13 @@
         <v>5</v>
       </c>
       <c r="D306" s="82" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="E306" s="56" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="F306" s="82" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="G306" s="69">
         <f>C306-0.0035</f>
@@ -8099,7 +8126,7 @@
       </c>
       <c r="D307" s="83"/>
       <c r="E307" s="56" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F307" s="83"/>
       <c r="G307" s="69">
@@ -8119,7 +8146,7 @@
       </c>
       <c r="D308" s="84"/>
       <c r="E308" s="56" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F308" s="84"/>
       <c r="G308" s="69">
@@ -8138,13 +8165,13 @@
         <v>100</v>
       </c>
       <c r="D309" s="69" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="E309" s="56" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="F309" s="69" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="G309" s="69">
         <f>C309-0.007</f>
@@ -8165,7 +8192,7 @@
     </row>
     <row r="311" spans="1:9" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A311" s="8" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B311" s="28"/>
       <c r="C311" s="28"/>
@@ -8178,7 +8205,7 @@
     </row>
     <row r="312" spans="1:9" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A312" s="8" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="B312" s="28"/>
       <c r="C312" s="28"/>
@@ -8191,18 +8218,18 @@
     </row>
     <row r="313" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A313" s="91" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B313" s="85" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="C313" s="86"/>
       <c r="D313" s="85" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="E313" s="86"/>
       <c r="F313" s="89" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="G313" s="90"/>
     </row>
@@ -8213,27 +8240,27 @@
       <c r="D314" s="87"/>
       <c r="E314" s="88"/>
       <c r="F314" s="58" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="G314" s="58" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="315" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A315" s="61" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="B315" s="61">
         <v>100</v>
       </c>
       <c r="C315" s="60" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="D315" s="57" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="E315" s="60" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="F315" s="15">
         <f>B315-0.01</f>
@@ -8246,19 +8273,19 @@
     </row>
     <row r="316" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A316" s="61" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="B316" s="61">
         <v>1</v>
       </c>
       <c r="C316" s="79" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="D316" s="57" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="E316" s="79" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="F316" s="64">
         <f>B316-0.000045</f>
@@ -8271,14 +8298,14 @@
     </row>
     <row r="317" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A317" s="61" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="B317" s="61">
         <v>10</v>
       </c>
       <c r="C317" s="80"/>
       <c r="D317" s="57" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="E317" s="80"/>
       <c r="F317" s="65">
@@ -8292,14 +8319,14 @@
     </row>
     <row r="318" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A318" s="32" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="B318" s="32">
         <v>100</v>
       </c>
       <c r="C318" s="81"/>
       <c r="D318" s="57" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="E318" s="81"/>
       <c r="F318" s="16">
@@ -8321,7 +8348,7 @@
     </row>
     <row r="320" spans="1:9" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A320" s="38" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="B320" s="28"/>
       <c r="C320" s="28"/>
@@ -8334,18 +8361,18 @@
     </row>
     <row r="321" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A321" s="91" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B321" s="85" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="C321" s="86"/>
       <c r="D321" s="85" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="E321" s="86"/>
       <c r="F321" s="89" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="G321" s="90"/>
     </row>
@@ -8356,27 +8383,27 @@
       <c r="D322" s="87"/>
       <c r="E322" s="88"/>
       <c r="F322" s="58" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="G322" s="58" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="323" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A323" s="61" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="B323" s="61">
         <v>1</v>
       </c>
       <c r="C323" s="95" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="D323" s="57" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="E323" s="95" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="F323" s="64">
         <f>B323-0.000075</f>
@@ -8389,14 +8416,14 @@
     </row>
     <row r="324" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A324" s="61" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="B324" s="61">
         <v>10</v>
       </c>
       <c r="C324" s="95"/>
       <c r="D324" s="57" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="E324" s="95"/>
       <c r="F324" s="16">
@@ -8410,14 +8437,14 @@
     </row>
     <row r="325" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A325" s="61" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="B325" s="61">
         <v>100</v>
       </c>
       <c r="C325" s="95"/>
       <c r="D325" s="57" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="E325" s="95"/>
       <c r="F325" s="19">
@@ -8431,19 +8458,19 @@
     </row>
     <row r="326" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A326" s="61" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="B326" s="61">
         <v>1</v>
       </c>
       <c r="C326" s="16" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D326" s="57" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="E326" s="16" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="F326" s="65">
         <f>B326-0.00301</f>
@@ -8467,23 +8494,23 @@
     </row>
     <row r="328" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A328" s="40" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="329" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A329" s="96" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B329" s="96" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C329" s="96"/>
       <c r="D329" s="96" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E329" s="96"/>
       <c r="F329" s="89" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="G329" s="90"/>
     </row>
@@ -8494,27 +8521,27 @@
       <c r="D330" s="96"/>
       <c r="E330" s="96"/>
       <c r="F330" s="58" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="G330" s="58" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="331" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A331" s="61" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="B331" s="61">
         <v>1</v>
       </c>
       <c r="C331" s="92" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="D331" s="57" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="E331" s="92" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="F331" s="15">
         <f>B331-0.01</f>
@@ -8527,14 +8554,14 @@
     </row>
     <row r="332" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A332" s="61" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="B332" s="61">
         <v>10</v>
       </c>
       <c r="C332" s="93"/>
       <c r="D332" s="57" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="E332" s="93"/>
       <c r="F332" s="15">
@@ -8548,14 +8575,14 @@
     </row>
     <row r="333" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A333" s="61" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="B333" s="61">
         <v>100</v>
       </c>
       <c r="C333" s="94"/>
       <c r="D333" s="57" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="E333" s="94"/>
       <c r="F333" s="19">
@@ -8569,19 +8596,19 @@
     </row>
     <row r="334" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A334" s="61" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="B334" s="61">
         <v>1</v>
       </c>
       <c r="C334" s="66" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="D334" s="57" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="E334" s="66" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="F334" s="18">
         <f>B334-0.005</f>
@@ -8599,47 +8626,63 @@
       <c r="D335" s="70"/>
       <c r="E335" s="25"/>
     </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A336" s="127" t="s">
+        <v>387</v>
+      </c>
+      <c r="B336" s="127"/>
+      <c r="C336" s="128" t="s">
+        <v>388</v>
+      </c>
+      <c r="D336" s="14"/>
+      <c r="E336" s="14"/>
+      <c r="F336" s="25"/>
+      <c r="I336" s="2"/>
+    </row>
+    <row r="337" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A337" s="127" t="s">
+        <v>330</v>
+      </c>
+      <c r="B337" s="127"/>
+      <c r="C337" s="41"/>
+      <c r="D337" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="E337" s="124" t="s">
+        <v>45</v>
+      </c>
+      <c r="F337" s="125"/>
+      <c r="G337" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H337" s="43"/>
+      <c r="I337" s="2"/>
+    </row>
+    <row r="338" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A338" s="127" t="s">
-        <v>327</v>
+        <v>15</v>
       </c>
       <c r="B338" s="127"/>
-      <c r="C338" s="41"/>
-      <c r="D338" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="E338" s="124" t="s">
-        <v>42</v>
-      </c>
-      <c r="F338" s="125"/>
-      <c r="G338" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="H338" s="43"/>
-    </row>
-    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A340" s="127" t="s">
-        <v>12</v>
-      </c>
-      <c r="B340" s="127"/>
-      <c r="C340" s="126" t="s">
-        <v>43</v>
-      </c>
-      <c r="D340" s="126"/>
+      <c r="C338" s="126" t="s">
+        <v>46</v>
+      </c>
+      <c r="D338" s="126"/>
+      <c r="I338" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="359">
+  <mergeCells count="360">
+    <mergeCell ref="A337:B337"/>
+    <mergeCell ref="E337:F337"/>
     <mergeCell ref="A215:A217"/>
     <mergeCell ref="B215:B217"/>
     <mergeCell ref="C215:C217"/>
     <mergeCell ref="F215:F217"/>
-    <mergeCell ref="E338:F338"/>
-    <mergeCell ref="C340:D340"/>
+    <mergeCell ref="C338:D338"/>
     <mergeCell ref="A201:A205"/>
     <mergeCell ref="A206:A210"/>
     <mergeCell ref="A213:A214"/>
-    <mergeCell ref="A340:B340"/>
     <mergeCell ref="A338:B338"/>
+    <mergeCell ref="A336:B336"/>
     <mergeCell ref="C230:C232"/>
     <mergeCell ref="F230:F232"/>
     <mergeCell ref="C245:C247"/>
@@ -8989,7 +9032,7 @@
     <mergeCell ref="G296:G297"/>
     <mergeCell ref="G286:G287"/>
   </mergeCells>
-  <pageMargins left="0.78740157480314965" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.39370078740157483"/>
+  <pageMargins left="0.78740157480314965" right="0.39370078740157483" top="0.39370078740157483" bottom="0.67708333333333337" header="0.39370078740157483" footer="0.39370078740157483"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;R&amp;"Times New Roman,обычный"&amp;P страница из &amp;N</oddFooter>

</xml_diff>